<commit_message>
Lots of updates, but everything seems to work now
</commit_message>
<xml_diff>
--- a/tests/cases_test.xlsx
+++ b/tests/cases_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Documents/_Plato/Plato/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C5833B-1383-C94C-ACFD-04915F6E2FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FD2A8C-FA84-1144-B9E2-BEA8B9A00A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" activeTab="1" xr2:uid="{0A9D0FCF-1F4B-5247-B35D-CBB46409C9D9}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>syn_ref</t>
+  </si>
+  <si>
+    <t>Depth-dependent mantle drag</t>
+  </si>
+  <si>
+    <t>LAB depth threshold</t>
+  </si>
+  <si>
+    <t>keels</t>
+  </si>
+  <si>
+    <t>syn_keels</t>
   </si>
 </sst>
 </file>
@@ -108,8 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,55 +533,115 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3288BC15-9473-3C46-93B5-57CBA9ED7537}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="b">
-        <v>0</v>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>150000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>